<commit_message>
Books have been added
</commit_message>
<xml_diff>
--- a/TCS NQT Schedule.xlsx
+++ b/TCS NQT Schedule.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhsingh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanisntsolo-boxx\Desktop\tcsSuperNinja\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB358A8-5582-4F02-8B46-11A9ACF96D85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -232,11 +233,14 @@
   <si>
     <t>RankingTest+MathmaticalOperations+PaperFolding+PaperCutting+7Codes</t>
   </si>
+  <si>
+    <t>4Codes+Non-verbal+Verbal Reasoning</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -533,41 +537,137 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -585,102 +685,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -967,11 +971,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21:R21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,36 +986,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="63" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="65"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="24"/>
     </row>
     <row r="2" spans="1:29" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A2" s="8" t="s">
@@ -1020,38 +1024,38 @@
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="67" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="57" t="s">
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="59" t="s">
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="60"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="28"/>
     </row>
     <row r="3" spans="1:29" ht="30.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="17">
@@ -1060,44 +1064,44 @@
       <c r="B3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
       <c r="H3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="39" t="s">
+      <c r="I3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="40"/>
-      <c r="S3" s="57" t="s">
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="58"/>
+      <c r="T3" s="26"/>
       <c r="U3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="W3" s="58" t="s">
+      <c r="W3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="58"/>
+      <c r="X3" s="26"/>
       <c r="Y3" s="10" t="s">
         <v>7</v>
       </c>
@@ -1112,44 +1116,44 @@
       <c r="B4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="39" t="s">
+      <c r="I4" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="49" t="s">
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="50"/>
+      <c r="T4" s="39"/>
       <c r="U4" s="12">
         <v>26</v>
       </c>
       <c r="V4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="W4" s="51" t="s">
+      <c r="W4" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="52"/>
+      <c r="X4" s="41"/>
       <c r="Y4" s="12">
         <v>10</v>
       </c>
@@ -1164,48 +1168,48 @@
       <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="39" t="s">
+      <c r="I5" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="49" t="s">
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="50"/>
+      <c r="T5" s="39"/>
       <c r="U5" s="12">
         <v>24</v>
       </c>
       <c r="V5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="W5" s="53" t="s">
+      <c r="W5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="53"/>
-      <c r="Y5" s="66">
+      <c r="X5" s="31"/>
+      <c r="Y5" s="32">
         <v>2</v>
       </c>
-      <c r="Z5" s="25" t="s">
+      <c r="Z5" s="33" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1216,40 +1220,40 @@
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="39" t="s">
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="26" t="s">
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="T6" s="27"/>
+      <c r="T6" s="30"/>
       <c r="U6" s="14">
         <v>30</v>
       </c>
       <c r="V6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="W6" s="53"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="66"/>
-      <c r="Z6" s="25"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="33"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
@@ -1261,43 +1265,43 @@
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="39" t="s">
+      <c r="I7" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="28" t="s">
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
       <c r="V7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
+      <c r="W7" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="37"/>
       <c r="Z7" s="16" t="s">
         <v>21</v>
       </c>
@@ -1309,30 +1313,30 @@
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
       <c r="H8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="39" t="s">
+      <c r="I8" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="40"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="49"/>
     </row>
     <row r="9" spans="1:29" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1341,30 +1345,30 @@
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
       <c r="H9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="41" t="s">
+      <c r="I9" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="43"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="47"/>
       <c r="S9" s="54" t="s">
         <v>29</v>
       </c>
@@ -1383,42 +1387,42 @@
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="41" t="s">
+      <c r="I10" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="57" t="s">
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="T10" s="58"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="58"/>
-      <c r="W10" s="59" t="s">
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="X10" s="59"/>
-      <c r="Y10" s="59"/>
-      <c r="Z10" s="60"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="28"/>
     </row>
     <row r="11" spans="1:29" ht="30.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
@@ -1427,44 +1431,44 @@
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="39" t="s">
+      <c r="I11" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="57" t="s">
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="T11" s="58"/>
+      <c r="T11" s="26"/>
       <c r="U11" s="10" t="s">
         <v>7</v>
       </c>
       <c r="V11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="W11" s="58" t="s">
+      <c r="W11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="X11" s="58"/>
+      <c r="X11" s="26"/>
       <c r="Y11" s="10" t="s">
         <v>7</v>
       </c>
@@ -1479,44 +1483,44 @@
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="39" t="s">
+      <c r="I12" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="49" t="s">
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="T12" s="50"/>
+      <c r="T12" s="39"/>
       <c r="U12" s="12">
         <v>15</v>
       </c>
       <c r="V12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="W12" s="51" t="s">
+      <c r="W12" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="X12" s="52"/>
+      <c r="X12" s="41"/>
       <c r="Y12" s="12">
         <v>10</v>
       </c>
@@ -1531,42 +1535,42 @@
       <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="49" t="s">
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="T13" s="50"/>
+      <c r="T13" s="39"/>
       <c r="U13" s="12">
         <v>20</v>
       </c>
       <c r="V13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="W13" s="53" t="s">
+      <c r="W13" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="X13" s="53"/>
-      <c r="Y13" s="24">
+      <c r="X13" s="31"/>
+      <c r="Y13" s="61">
         <v>2</v>
       </c>
-      <c r="Z13" s="25" t="s">
+      <c r="Z13" s="33" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1577,44 +1581,44 @@
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="42" t="s">
+      <c r="I14" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="26" t="s">
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="T14" s="27"/>
+      <c r="T14" s="30"/>
       <c r="U14" s="14">
         <v>15</v>
       </c>
       <c r="V14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="W14" s="53"/>
-      <c r="X14" s="53"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="25"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="61"/>
+      <c r="Z14" s="33"/>
     </row>
     <row r="15" spans="1:29" ht="30.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="1">
@@ -1623,43 +1627,43 @@
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="42" t="s">
+      <c r="I15" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="28" t="s">
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
       <c r="V15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="W15" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="31"/>
+      <c r="W15" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
       <c r="Z15" s="16" t="s">
         <v>21</v>
       </c>
@@ -1671,40 +1675,40 @@
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="41" t="s">
+      <c r="I16" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="32" t="s">
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="T16" s="33"/>
-      <c r="U16" s="33"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
-      <c r="X16" s="33"/>
-      <c r="Y16" s="33"/>
-      <c r="Z16" s="33"/>
+      <c r="T16" s="65"/>
+      <c r="U16" s="65"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="65"/>
+      <c r="X16" s="65"/>
+      <c r="Y16" s="65"/>
+      <c r="Z16" s="65"/>
     </row>
     <row r="17" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -1713,38 +1717,38 @@
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
       <c r="H17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="68" t="s">
+      <c r="I17" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="N17" s="68"/>
-      <c r="O17" s="68"/>
-      <c r="P17" s="68"/>
-      <c r="Q17" s="68"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="35"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="67"/>
+      <c r="U17" s="67"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="67"/>
+      <c r="X17" s="67"/>
+      <c r="Y17" s="67"/>
+      <c r="Z17" s="67"/>
     </row>
     <row r="18" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -1753,38 +1757,38 @@
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
       <c r="H18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="68" t="s">
+      <c r="I18" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="N18" s="68"/>
-      <c r="O18" s="68"/>
-      <c r="P18" s="68"/>
-      <c r="Q18" s="68"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="35"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="67"/>
+      <c r="U18" s="67"/>
+      <c r="V18" s="67"/>
+      <c r="W18" s="67"/>
+      <c r="X18" s="67"/>
+      <c r="Y18" s="67"/>
+      <c r="Z18" s="67"/>
     </row>
     <row r="19" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -1793,38 +1797,38 @@
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
       <c r="H19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="68" t="s">
+      <c r="I19" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="N19" s="68"/>
-      <c r="O19" s="68"/>
-      <c r="P19" s="68"/>
-      <c r="Q19" s="68"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
-      <c r="Y19" s="35"/>
-      <c r="Z19" s="35"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="62"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="67"/>
+      <c r="U19" s="67"/>
+      <c r="V19" s="67"/>
+      <c r="W19" s="67"/>
+      <c r="X19" s="67"/>
+      <c r="Y19" s="67"/>
+      <c r="Z19" s="67"/>
     </row>
     <row r="20" spans="1:26" s="6" customFormat="1" ht="30.15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A20" s="3">
@@ -1833,34 +1837,34 @@
       <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="69" t="s">
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="N20" s="68"/>
-      <c r="O20" s="68"/>
-      <c r="P20" s="68"/>
-      <c r="Q20" s="68"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
-      <c r="X20" s="35"/>
-      <c r="Y20" s="35"/>
-      <c r="Z20" s="35"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="67"/>
+      <c r="U20" s="67"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="67"/>
+      <c r="X20" s="67"/>
+      <c r="Y20" s="67"/>
+      <c r="Z20" s="67"/>
     </row>
     <row r="21" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -1869,38 +1873,38 @@
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
       <c r="H21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="68"/>
-      <c r="P21" s="68"/>
-      <c r="Q21" s="68"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="36" t="s">
+      <c r="I21" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="62"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="37"/>
+      <c r="T21" s="69"/>
+      <c r="U21" s="69"/>
+      <c r="V21" s="69"/>
+      <c r="W21" s="69"/>
+      <c r="X21" s="69"/>
+      <c r="Y21" s="69"/>
+      <c r="Z21" s="69"/>
     </row>
     <row r="22" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1909,36 +1913,36 @@
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
       <c r="H22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="37"/>
-      <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="37"/>
+      <c r="I22" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="53"/>
+      <c r="S22" s="68"/>
+      <c r="T22" s="69"/>
+      <c r="U22" s="69"/>
+      <c r="V22" s="69"/>
+      <c r="W22" s="69"/>
+      <c r="X22" s="69"/>
+      <c r="Y22" s="69"/>
+      <c r="Z22" s="69"/>
     </row>
     <row r="23" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -1947,36 +1951,38 @@
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="37"/>
+      <c r="I23" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="68"/>
+      <c r="T23" s="69"/>
+      <c r="U23" s="69"/>
+      <c r="V23" s="69"/>
+      <c r="W23" s="69"/>
+      <c r="X23" s="69"/>
+      <c r="Y23" s="69"/>
+      <c r="Z23" s="69"/>
     </row>
     <row r="24" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1985,36 +1991,36 @@
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
       <c r="H24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="37"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="37"/>
-      <c r="Z24" s="37"/>
+      <c r="I24" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="68"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="69"/>
+      <c r="V24" s="69"/>
+      <c r="W24" s="69"/>
+      <c r="X24" s="69"/>
+      <c r="Y24" s="69"/>
+      <c r="Z24" s="69"/>
     </row>
     <row r="25" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -2023,36 +2029,36 @@
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
       <c r="H25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="37"/>
-      <c r="U25" s="37"/>
-      <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
-      <c r="X25" s="37"/>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="37"/>
+      <c r="I25" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="52"/>
+      <c r="P25" s="52"/>
+      <c r="Q25" s="52"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="68"/>
+      <c r="T25" s="69"/>
+      <c r="U25" s="69"/>
+      <c r="V25" s="69"/>
+      <c r="W25" s="69"/>
+      <c r="X25" s="69"/>
+      <c r="Y25" s="69"/>
+      <c r="Z25" s="69"/>
     </row>
     <row r="26" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -2061,36 +2067,36 @@
       <c r="B26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
       <c r="H26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="37"/>
-      <c r="U26" s="37"/>
-      <c r="V26" s="37"/>
-      <c r="W26" s="37"/>
-      <c r="X26" s="37"/>
-      <c r="Y26" s="37"/>
-      <c r="Z26" s="37"/>
+      <c r="I26" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="52"/>
+      <c r="P26" s="52"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="68"/>
+      <c r="T26" s="69"/>
+      <c r="U26" s="69"/>
+      <c r="V26" s="69"/>
+      <c r="W26" s="69"/>
+      <c r="X26" s="69"/>
+      <c r="Y26" s="69"/>
+      <c r="Z26" s="69"/>
     </row>
     <row r="27" spans="1:26" s="6" customFormat="1" ht="30.15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A27" s="3">
@@ -2099,32 +2105,32 @@
       <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="37"/>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="37"/>
-      <c r="Z27" s="37"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="68"/>
+      <c r="T27" s="69"/>
+      <c r="U27" s="69"/>
+      <c r="V27" s="69"/>
+      <c r="W27" s="69"/>
+      <c r="X27" s="69"/>
+      <c r="Y27" s="69"/>
+      <c r="Z27" s="69"/>
     </row>
     <row r="28" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -2133,28 +2139,28 @@
       <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
       <c r="H28" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="23"/>
+      <c r="I28" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="53"/>
     </row>
     <row r="29" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -2163,28 +2169,28 @@
       <c r="B29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
       <c r="H29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="23"/>
+      <c r="I29" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="53"/>
     </row>
     <row r="30" spans="1:26" ht="30.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -2193,49 +2199,102 @@
       <c r="B30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
       <c r="H30" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="23"/>
+      <c r="I30" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="52"/>
+      <c r="Q30" s="52"/>
+      <c r="R30" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="S1:Z1"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="W5:X6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="W7:Y7"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="C20:L20"/>
+    <mergeCell ref="M30:R30"/>
+    <mergeCell ref="M22:R22"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="Y13:Y14"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="M28:R28"/>
+    <mergeCell ref="M23:R23"/>
+    <mergeCell ref="M24:R24"/>
+    <mergeCell ref="M25:R25"/>
+    <mergeCell ref="M26:R26"/>
+    <mergeCell ref="M27:R27"/>
+    <mergeCell ref="M16:R16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="M18:R18"/>
+    <mergeCell ref="M19:R19"/>
+    <mergeCell ref="M20:R20"/>
+    <mergeCell ref="M21:R21"/>
+    <mergeCell ref="S16:Z20"/>
+    <mergeCell ref="S21:Z27"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="I30:L30"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="M7:R7"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="C27:L27"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="I10:L10"/>
     <mergeCell ref="S12:T12"/>
     <mergeCell ref="W12:X12"/>
     <mergeCell ref="M10:R10"/>
@@ -2260,77 +2319,24 @@
     <mergeCell ref="I7:L7"/>
     <mergeCell ref="I8:L8"/>
     <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C27:L27"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="I30:L30"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="M4:R4"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="M6:R6"/>
-    <mergeCell ref="M7:R7"/>
-    <mergeCell ref="M8:R8"/>
-    <mergeCell ref="M9:R9"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="I22:L22"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="M30:R30"/>
-    <mergeCell ref="M22:R22"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="Y13:Y14"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="M28:R28"/>
-    <mergeCell ref="M23:R23"/>
-    <mergeCell ref="M24:R24"/>
-    <mergeCell ref="M25:R25"/>
-    <mergeCell ref="M26:R26"/>
-    <mergeCell ref="M27:R27"/>
-    <mergeCell ref="M16:R16"/>
-    <mergeCell ref="M17:R17"/>
-    <mergeCell ref="M18:R18"/>
-    <mergeCell ref="M19:R19"/>
-    <mergeCell ref="M20:R20"/>
-    <mergeCell ref="M21:R21"/>
-    <mergeCell ref="S16:Z20"/>
-    <mergeCell ref="S21:Z27"/>
-    <mergeCell ref="C20:L20"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="S1:Z1"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="W5:X6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>